<commit_message>
optimized images and minified JS/CSS
</commit_message>
<xml_diff>
--- a/P4/Template+SEO+analysis.xlsx
+++ b/P4/Template+SEO+analysis.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Category</t>
   </si>
@@ -59,6 +59,43 @@
   </si>
   <si>
     <t>MFI</t>
+  </si>
+  <si>
+    <t>Images weights too much</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Images weight should be optimized in order to reduce the weight  and the MB of the webpages. 
+</t>
+  </si>
+  <si>
+    <t>Reduce the weight of the images using a optimizer like the google app squoosh.app</t>
+  </si>
+  <si>
+    <t>Images format</t>
+  </si>
+  <si>
+    <t>The images format is not the correct one</t>
+  </si>
+  <si>
+    <t>Converting the bmp to jpg</t>
+  </si>
+  <si>
+    <t>Images size</t>
+  </si>
+  <si>
+    <t>The images should be proprerly sized in order to optimize the pages speed.</t>
+  </si>
+  <si>
+    <t>Properly size the images</t>
+  </si>
+  <si>
+    <t>Minify JS and CSS</t>
+  </si>
+  <si>
+    <t>Minify the CSS and JS is a simply action which will have impact on the page speed,</t>
+  </si>
+  <si>
+    <t>Minify CSS and JS</t>
   </si>
 </sst>
 </file>
@@ -66,10 +103,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -103,9 +140,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -142,14 +186,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -157,14 +193,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -178,15 +214,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -217,15 +262,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -268,37 +305,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -310,7 +455,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -323,126 +480,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -453,80 +490,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -549,6 +512,80 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
@@ -556,156 +593,161 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1026,78 +1068,124 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelRow="6" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="35" customWidth="1"/>
-    <col min="4" max="4" width="43.3333333333333" customWidth="1"/>
-    <col min="5" max="5" width="43.8333333333333" customWidth="1"/>
-    <col min="6" max="6" width="21" customWidth="1"/>
+    <col min="1" max="1" width="27" style="2" customWidth="1"/>
+    <col min="2" max="2" width="35" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11" style="2"/>
+    <col min="4" max="4" width="43.3333333333333" style="2" customWidth="1"/>
+    <col min="5" max="5" width="43.8333333333333" style="2" customWidth="1"/>
+    <col min="6" max="6" width="21" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:6">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="2:2">
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:2">
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="2:2">
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="2:2">
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="2:2">
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="8" ht="46.8" spans="2:5">
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="B9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" ht="31.2" spans="2:5">
+      <c r="B10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" ht="31.2" spans="2:5">
+      <c r="B11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>